<commit_message>
version 1 is ready. 3 doctors and continuous update.
</commit_message>
<xml_diff>
--- a/galilean.xlsx
+++ b/galilean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspace\EREZ\galilean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A641F0D-2F49-42C8-8EAE-E4E0AA467B85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069D5997-AB72-481A-BC09-320994D5EF52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{478A9EFA-3F6C-41E7-929E-7486A48D12FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{478A9EFA-3F6C-41E7-929E-7486A48D12FC}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>cycle</t>
+  </si>
+  <si>
+    <t>steve</t>
   </si>
 </sst>
 </file>
@@ -867,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD86E69-7CBE-4FA3-9342-B303AB23BBBD}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,10 +975,16 @@
       <c r="A8" s="4">
         <v>14</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1627,7 +1636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C11AFBD5-2DA8-4BE1-B59C-3E6B83201776}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1650,7 +1659,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>1000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding more images and updating readme files.
</commit_message>
<xml_diff>
--- a/galilean.xlsx
+++ b/galilean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspace\EREZ\galilean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069D5997-AB72-481A-BC09-320994D5EF52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F286AE1-0066-4A93-AC1F-71C04C96B33A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{478A9EFA-3F6C-41E7-929E-7486A48D12FC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -871,7 +871,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1041,9 @@
       <c r="A14" s="5">
         <v>20</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>2</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>

</xml_diff>

<commit_message>
version 2 - server mode added, both working.
</commit_message>
<xml_diff>
--- a/galilean.xlsx
+++ b/galilean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspace\EREZ\galilean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F286AE1-0066-4A93-AC1F-71C04C96B33A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE01CD35-67A0-46D6-B8A2-300E866D5AF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{478A9EFA-3F6C-41E7-929E-7486A48D12FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{478A9EFA-3F6C-41E7-929E-7486A48D12FC}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD86E69-7CBE-4FA3-9342-B303AB23BBBD}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,8 +992,12 @@
         <v>15</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
@@ -1260,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A06901-18A1-4B75-8434-832CA8B8F9F9}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,8 +1382,12 @@
         <v>15</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
@@ -1417,9 +1425,13 @@
       <c r="A13" s="4">
         <v>19</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
@@ -1428,18 +1440,37 @@
         <v>20</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="10">
+        <v>21</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1639,7 +1670,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,6 +1699,9 @@
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B3" s="2">
+        <v>2000</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">

</xml_diff>